<commit_message>
added nr cylces column
</commit_message>
<xml_diff>
--- a/Project Lab/Timing&Util data.xlsx
+++ b/Project Lab/Timing&Util data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugof\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugof\Documents\KU Leuven\FIIW\BAC3\Complex Digital Design\Project Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10524B8B-5F93-4B6A-9D87-EA5EF6B64CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5C2EFD-0922-4422-8AF8-0B4C0360ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D6DAB14B-4605-4031-9EB2-11B8E4E1523A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>RCA</t>
   </si>
@@ -77,7 +77,13 @@
     <t>Applied Formatting Rules</t>
   </si>
   <si>
-    <t>WNS for CSelLa only depends on Block Size -&gt; Normal??</t>
+    <t>TODO: data for CSelA</t>
+  </si>
+  <si>
+    <t>Nr Cycles</t>
+  </si>
+  <si>
+    <t>OPERAND_WIDTH</t>
   </si>
 </sst>
 </file>
@@ -319,11 +325,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -332,11 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -347,19 +347,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -405,16 +440,23 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9400D3"/>
+        <color rgb="FFFF0000"/>
       </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -424,32 +466,6 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -462,59 +478,14 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -522,13 +493,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -546,9 +510,25 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -556,69 +536,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -959,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13F0340-F4D3-442E-ACFB-CC8403AD3F2D}">
-  <dimension ref="B1:I35"/>
+  <dimension ref="B1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,14 +891,14 @@
     <col min="6" max="7" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -997,619 +914,755 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>16</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>2.5329999999999999</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>1073</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="4">
         <v>1573</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="5">
+        <f>$J$2/C2+2</f>
+        <v>34</v>
+      </c>
+      <c r="J2" s="21">
+        <v>512</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>32</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>-1.484</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>1081</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>1571</v>
       </c>
-      <c r="I3" s="17">
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H33" si="0">$J$2/C3+2</f>
+        <v>18</v>
+      </c>
+      <c r="K3" s="11">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>16</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>2.653</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1066</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>1571</v>
       </c>
-      <c r="I4" s="18">
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="K4" s="12">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="22">
         <v>32</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="22">
         <v>3.1840000000000002</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="22">
         <v>1173</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="22">
         <v>1569</v>
       </c>
-      <c r="I5" s="19">
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K5" s="13">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="22">
         <v>64</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="22">
         <v>2.1019999999999999</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="22">
         <v>1453</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="22">
         <v>1571</v>
       </c>
-      <c r="I6" s="20">
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K6" s="14">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>128</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>1.0129999999999999</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>2051</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <v>1570</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
         <v>16</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="13">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="22">
         <v>32</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="22">
         <v>4</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="13">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="22">
         <v>32</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="22">
         <v>8</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="13">
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="22">
         <v>32</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="22">
         <v>16</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="13">
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="22">
         <v>64</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="22">
         <v>4</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="13">
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="22">
         <v>64</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="22">
         <v>8</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="13">
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="22">
         <v>64</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="22">
         <v>16</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="13">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="22">
         <v>64</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="22">
         <v>32</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="13">
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="22">
         <v>128</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="22">
         <v>4</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="13">
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="22">
         <v>128</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="22">
         <v>8</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="13">
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="22">
         <v>128</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="22">
         <v>16</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="13">
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="22">
         <v>128</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="22">
         <v>32</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9">
         <v>128</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>64</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="22">
         <v>16</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="22">
         <v>4</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="22">
         <v>5.4470000000000001</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="22">
         <v>1071</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="22">
         <v>1579</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="7" t="s">
+      <c r="H21" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="22">
         <v>32</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="22">
         <v>4</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="22">
         <v>5.5289999999999999</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="22">
         <v>1061</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="22">
         <v>1571</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="7" t="s">
+      <c r="H22" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="22">
         <v>32</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="22">
         <v>8</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="22">
         <v>4.4740000000000002</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="22">
         <v>1081</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="22">
         <v>1578</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="7" t="s">
+      <c r="H23" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="22">
         <v>32</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="22">
         <v>16</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="22">
         <v>2.218</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="22">
         <v>1088</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="22">
         <v>1570</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="7" t="s">
+      <c r="H24" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="22">
         <v>64</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="22">
         <v>4</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="22">
         <v>5.5289999999999999</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="22">
         <v>1073</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="22">
         <v>1578</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="7" t="s">
+      <c r="H25" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="22">
         <v>64</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="22">
         <v>8</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="22">
         <v>4.4749999999999996</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="22">
         <v>1081</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="22">
         <v>1568</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
+      <c r="H26" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="22">
         <v>64</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="22">
         <v>16</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="22">
         <v>2.218</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="22">
         <v>1136</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="22">
         <v>1569</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="7" t="s">
+      <c r="H27" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="22">
         <v>64</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="22">
         <v>32</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="22">
         <v>2.383</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="22">
         <v>1318</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="22">
         <v>1568</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="7" t="s">
+      <c r="H28" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="22">
         <v>128</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="22">
         <v>4</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="22">
         <v>5.5289999999999999</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="22">
         <v>1061</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="22">
         <v>1568</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="7" t="s">
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="22">
         <v>128</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="22">
         <v>8</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="22">
         <v>4.4749999999999996</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="22">
         <v>1116</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="22">
         <v>1576</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="7" t="s">
+      <c r="H30" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="22">
         <v>128</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="22">
         <v>16</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="22">
         <v>2.218</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="22">
         <v>1218</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="22">
         <v>1560</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="7" t="s">
+      <c r="H31" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="22">
         <v>128</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="22">
         <v>32</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="22">
         <v>2.383</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="22">
         <v>1629</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="22">
         <v>1567</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="9" t="s">
+      <c r="H32" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>128</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <v>64</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>1.008</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="9">
         <v>1865</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="9">
         <v>1568</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B35" s="26" t="s">
+      <c r="H33" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="19" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B2:G33 B35">
-    <cfRule type="expression" dxfId="5" priority="3">
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="top10" dxfId="11" priority="1" rank="1"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:H33">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>$C2=128</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$C2=64</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$C2=32</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$C2=16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E33">
-    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
-      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated excel with CSelA and CSelLA values
</commit_message>
<xml_diff>
--- a/Project Lab/Timing&Util data.xlsx
+++ b/Project Lab/Timing&Util data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugof\Documents\KU Leuven\FIIW\BAC3\Complex Digital Design\Project Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5C2EFD-0922-4422-8AF8-0B4C0360ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D9AAC2-4FCC-4323-A2D6-8675B58B2126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D6DAB14B-4605-4031-9EB2-11B8E4E1523A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>RCA</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Applied Formatting Rules</t>
   </si>
   <si>
-    <t>TODO: data for CSelA</t>
-  </si>
-  <si>
     <t>Nr Cycles</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,155 +347,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -876,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13F0340-F4D3-442E-ACFB-CC8403AD3F2D}">
-  <dimension ref="B1:K36"/>
+  <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,8 +764,9 @@
     <col min="6" max="7" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
     <col min="11" max="11" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.90625" bestFit="1" customWidth="1"/>
@@ -917,13 +791,13 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -950,10 +824,10 @@
         <f>$J$2/C2+2</f>
         <v>34</v>
       </c>
-      <c r="J2" s="21">
+      <c r="J2" s="19">
         <v>512</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1015,19 +889,19 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5">
         <v>32</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5">
         <v>3.1840000000000002</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5">
         <v>1173</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5">
         <v>1569</v>
       </c>
       <c r="H5" s="7">
@@ -1042,19 +916,19 @@
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6">
         <v>64</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6">
         <v>2.1019999999999999</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6">
         <v>1453</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6">
         <v>1571</v>
       </c>
       <c r="H6" s="7">
@@ -1088,7 +962,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="25" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1102,9 +976,15 @@
       <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="E8" s="4">
+        <v>3.6779999999999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1084</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1579</v>
+      </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1114,15 +994,21 @@
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9">
         <v>32</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="E9" s="23">
+        <v>2.468</v>
+      </c>
+      <c r="F9" s="23">
+        <v>1089</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1570</v>
+      </c>
       <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1132,15 +1018,21 @@
       <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10">
         <v>32</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="E10" s="23">
+        <v>2.4910000000000001</v>
+      </c>
+      <c r="F10" s="23">
+        <v>1092</v>
+      </c>
+      <c r="G10" s="23">
+        <v>1579</v>
+      </c>
       <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1150,15 +1042,21 @@
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11">
         <v>32</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11">
         <v>16</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="E11" s="23">
+        <v>1.5309999999999999</v>
+      </c>
+      <c r="F11" s="23">
+        <v>1095</v>
+      </c>
+      <c r="G11" s="23">
+        <v>1582</v>
+      </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1168,15 +1066,21 @@
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12">
         <v>64</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
+      <c r="E12" s="23">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <v>1112</v>
+      </c>
+      <c r="G12" s="23">
+        <v>1570</v>
+      </c>
       <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1186,15 +1090,21 @@
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13">
         <v>64</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13">
         <v>8</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="E13" s="23">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="F13" s="23">
+        <v>1112</v>
+      </c>
+      <c r="G13" s="23">
+        <v>1569</v>
+      </c>
       <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1204,15 +1114,21 @@
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14">
         <v>64</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14">
         <v>16</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
+      <c r="E14" s="23">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="F14" s="23">
+        <v>1139</v>
+      </c>
+      <c r="G14" s="23">
+        <v>1571</v>
+      </c>
       <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1222,15 +1138,21 @@
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15">
         <v>64</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15">
         <v>32</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="E15" s="23">
+        <v>-1.919</v>
+      </c>
+      <c r="F15" s="23">
+        <v>1162</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1570</v>
+      </c>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1240,15 +1162,21 @@
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16">
         <v>128</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16">
         <v>4</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="E16" s="23">
+        <v>-4.7919999999999998</v>
+      </c>
+      <c r="F16" s="23">
+        <v>1180</v>
+      </c>
+      <c r="G16" s="23">
+        <v>1576</v>
+      </c>
       <c r="H16" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1258,15 +1186,21 @@
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17">
         <v>128</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17">
         <v>8</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
+      <c r="E17" s="23">
+        <v>-1.2130000000000001</v>
+      </c>
+      <c r="F17" s="23">
+        <v>1189</v>
+      </c>
+      <c r="G17" s="23">
+        <v>1569</v>
+      </c>
       <c r="H17" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1276,15 +1210,21 @@
       <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18">
         <v>128</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18">
         <v>16</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
+      <c r="E18" s="23">
+        <v>-0.95199999999999996</v>
+      </c>
+      <c r="F18" s="23">
+        <v>1196</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1568</v>
+      </c>
       <c r="H18" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1294,15 +1234,21 @@
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19">
         <v>128</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19">
         <v>32</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
+      <c r="E19" s="24">
+        <v>-2.96</v>
+      </c>
+      <c r="F19" s="23">
+        <v>1280</v>
+      </c>
+      <c r="G19" s="23">
+        <v>1571</v>
+      </c>
       <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1318,9 +1264,15 @@
       <c r="D20" s="9">
         <v>64</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="E20" s="9">
+        <v>-10.045999999999999</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1251</v>
+      </c>
+      <c r="G20" s="9">
+        <v>1572</v>
+      </c>
       <c r="H20" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1330,20 +1282,20 @@
       <c r="B21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21">
         <v>16</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21">
         <v>4</v>
       </c>
-      <c r="E21" s="22">
-        <v>5.4470000000000001</v>
-      </c>
-      <c r="F21" s="22">
-        <v>1071</v>
-      </c>
-      <c r="G21" s="22">
-        <v>1579</v>
+      <c r="E21" s="23">
+        <v>3.415</v>
+      </c>
+      <c r="F21" s="23">
+        <v>1081</v>
+      </c>
+      <c r="G21" s="23">
+        <v>1575</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" si="0"/>
@@ -1354,20 +1306,20 @@
       <c r="B22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22">
         <v>32</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22">
         <v>4</v>
       </c>
-      <c r="E22" s="22">
-        <v>5.5289999999999999</v>
-      </c>
-      <c r="F22" s="22">
-        <v>1061</v>
-      </c>
-      <c r="G22" s="22">
-        <v>1571</v>
+      <c r="E22" s="23">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="F22" s="23">
+        <v>1078</v>
+      </c>
+      <c r="G22" s="23">
+        <v>1555</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="0"/>
@@ -1378,20 +1330,20 @@
       <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23">
         <v>32</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23">
         <v>8</v>
       </c>
-      <c r="E23" s="22">
-        <v>4.4740000000000002</v>
-      </c>
-      <c r="F23" s="22">
-        <v>1081</v>
-      </c>
-      <c r="G23" s="22">
-        <v>1578</v>
+      <c r="E23" s="23">
+        <v>2.8690000000000002</v>
+      </c>
+      <c r="F23" s="23">
+        <v>1122</v>
+      </c>
+      <c r="G23" s="23">
+        <v>1574</v>
       </c>
       <c r="H23" s="7">
         <f t="shared" si="0"/>
@@ -1402,20 +1354,20 @@
       <c r="B24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24">
         <v>32</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24">
         <v>16</v>
       </c>
-      <c r="E24" s="22">
-        <v>2.218</v>
-      </c>
-      <c r="F24" s="22">
-        <v>1088</v>
-      </c>
-      <c r="G24" s="22">
-        <v>1570</v>
+      <c r="E24" s="23">
+        <v>2.9239999999999999</v>
+      </c>
+      <c r="F24" s="23">
+        <v>1142</v>
+      </c>
+      <c r="G24" s="23">
+        <v>1573</v>
       </c>
       <c r="H24" s="7">
         <f t="shared" si="0"/>
@@ -1426,20 +1378,20 @@
       <c r="B25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25">
         <v>64</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25">
         <v>4</v>
       </c>
-      <c r="E25" s="22">
-        <v>5.5289999999999999</v>
-      </c>
-      <c r="F25" s="22">
-        <v>1073</v>
-      </c>
-      <c r="G25" s="22">
-        <v>1578</v>
+      <c r="E25" s="23">
+        <v>0.876</v>
+      </c>
+      <c r="F25" s="23">
+        <v>1112</v>
+      </c>
+      <c r="G25" s="23">
+        <v>1569</v>
       </c>
       <c r="H25" s="7">
         <f t="shared" si="0"/>
@@ -1450,20 +1402,20 @@
       <c r="B26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26">
         <v>64</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26">
         <v>8</v>
       </c>
-      <c r="E26" s="22">
-        <v>4.4749999999999996</v>
-      </c>
-      <c r="F26" s="22">
-        <v>1081</v>
-      </c>
-      <c r="G26" s="22">
-        <v>1568</v>
+      <c r="E26" s="23">
+        <v>1.7709999999999999</v>
+      </c>
+      <c r="F26" s="23">
+        <v>1127</v>
+      </c>
+      <c r="G26" s="23">
+        <v>1564</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" si="0"/>
@@ -1474,19 +1426,19 @@
       <c r="B27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27">
         <v>64</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27">
         <v>16</v>
       </c>
-      <c r="E27" s="22">
-        <v>2.218</v>
-      </c>
-      <c r="F27" s="22">
-        <v>1136</v>
-      </c>
-      <c r="G27" s="22">
+      <c r="E27" s="23">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="F27" s="23">
+        <v>1142</v>
+      </c>
+      <c r="G27" s="23">
         <v>1569</v>
       </c>
       <c r="H27" s="7">
@@ -1498,20 +1450,20 @@
       <c r="B28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28">
         <v>64</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28">
         <v>32</v>
       </c>
-      <c r="E28" s="22">
-        <v>2.383</v>
-      </c>
-      <c r="F28" s="22">
-        <v>1318</v>
-      </c>
-      <c r="G28" s="22">
-        <v>1568</v>
+      <c r="E28" s="23">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="F28" s="23">
+        <v>1455</v>
+      </c>
+      <c r="G28" s="23">
+        <v>1570</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
@@ -1522,20 +1474,20 @@
       <c r="B29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29">
         <v>128</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29">
         <v>4</v>
       </c>
-      <c r="E29" s="22">
-        <v>5.5289999999999999</v>
-      </c>
-      <c r="F29" s="22">
-        <v>1061</v>
-      </c>
-      <c r="G29" s="22">
-        <v>1568</v>
+      <c r="E29" s="23">
+        <v>-2.681</v>
+      </c>
+      <c r="F29" s="23">
+        <v>1170</v>
+      </c>
+      <c r="G29" s="23">
+        <v>1566</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" si="0"/>
@@ -1546,20 +1498,20 @@
       <c r="B30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30">
         <v>128</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30">
         <v>8</v>
       </c>
-      <c r="E30" s="22">
-        <v>4.4749999999999996</v>
-      </c>
-      <c r="F30" s="22">
-        <v>1116</v>
-      </c>
-      <c r="G30" s="22">
-        <v>1576</v>
+      <c r="E30" s="23">
+        <v>-0.91500000000000004</v>
+      </c>
+      <c r="F30" s="23">
+        <v>1187</v>
+      </c>
+      <c r="G30" s="23">
+        <v>1569</v>
       </c>
       <c r="H30" s="7">
         <f t="shared" si="0"/>
@@ -1570,20 +1522,20 @@
       <c r="B31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31">
         <v>128</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31">
         <v>16</v>
       </c>
-      <c r="E31" s="22">
-        <v>2.218</v>
-      </c>
-      <c r="F31" s="22">
-        <v>1218</v>
-      </c>
-      <c r="G31" s="22">
-        <v>1560</v>
+      <c r="E31" s="23">
+        <v>-0.92100000000000004</v>
+      </c>
+      <c r="F31" s="23">
+        <v>1204</v>
+      </c>
+      <c r="G31" s="23">
+        <v>1568</v>
       </c>
       <c r="H31" s="7">
         <f t="shared" si="0"/>
@@ -1594,20 +1546,20 @@
       <c r="B32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32">
         <v>128</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32">
         <v>32</v>
       </c>
-      <c r="E32" s="22">
-        <v>2.383</v>
-      </c>
-      <c r="F32" s="22">
-        <v>1629</v>
-      </c>
-      <c r="G32" s="22">
-        <v>1567</v>
+      <c r="E32" s="23">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="F32" s="23">
+        <v>1989</v>
+      </c>
+      <c r="G32" s="23">
+        <v>1570</v>
       </c>
       <c r="H32" s="7">
         <f t="shared" si="0"/>
@@ -1625,44 +1577,39 @@
         <v>64</v>
       </c>
       <c r="E33" s="9">
-        <v>1.008</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="F33" s="9">
-        <v>1865</v>
+        <v>2183</v>
       </c>
       <c r="G33" s="9">
-        <v>1568</v>
+        <v>1573</v>
       </c>
       <c r="H33" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B36" s="19" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E33">
-    <cfRule type="top10" dxfId="11" priority="1" rank="1"/>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
-      <formula>0</formula>
+  <conditionalFormatting sqref="B2:H33">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>$C2=128</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>$C2=64</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>$C2=32</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>$C2=16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H33">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>$C2=128</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$C2=64</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$C2=32</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$C2=16</formula>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>